<commit_message>
fixing visuals that were broken
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week2.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week2.xlsx
@@ -887,40 +887,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>UL Monroe</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3.3</v>
+        <v>7.1</v>
       </c>
       <c r="E10" t="n">
-        <v>7.600000000000001</v>
+        <v>7.9</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Alabama -36.5</t>
+          <t>Tulane -10.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Alabama -36.5</t>
+          <t>Tulane -10.5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Alabama -44.1</t>
+          <t>Tulane -2.6</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>44.1</v>
+        <v>-2.6</v>
       </c>
       <c r="J10" t="n">
-        <v>36.5</v>
+        <v>-10.5</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -934,40 +934,40 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>UL Monroe</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="E11" t="n">
         <v>7.600000000000001</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Pittsburgh -21.5</t>
+          <t>Alabama -36.5</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Pittsburgh -21.5</t>
+          <t>Alabama -36.5</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Pittsburgh -29.1</t>
+          <t>Alabama -44.1</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>29.1</v>
+        <v>44.1</v>
       </c>
       <c r="J11" t="n">
-        <v>21.5</v>
+        <v>36.5</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -981,40 +981,40 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7.1</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>6.9</v>
+        <v>7.600000000000001</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Tulane -10.5</t>
+          <t>Pittsburgh -21.5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Tulane -9.5</t>
+          <t>Pittsburgh -21.5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Tulane -2.6</t>
+          <t>Pittsburgh -29.1</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>-2.6</v>
+        <v>29.1</v>
       </c>
       <c r="J12" t="n">
-        <v>-9.5</v>
+        <v>21.5</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -2062,40 +2062,40 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>New Mexico State</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3.6</v>
+        <v>4.6</v>
       </c>
       <c r="E35" t="n">
-        <v>3.4</v>
+        <v>3.200000000000003</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Tulsa -3.5</t>
+          <t>Texas A&amp;M -30.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Tulsa -3.5</t>
+          <t>Texas A&amp;M -29.5</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Tulsa -6.9</t>
+          <t>Texas A&amp;M -32.7</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>-6.9</v>
+        <v>32.7</v>
       </c>
       <c r="J35" t="n">
-        <v>-3.5</v>
+        <v>29.5</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -2109,40 +2109,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Army</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4.6</v>
+        <v>6.2</v>
       </c>
       <c r="E36" t="n">
-        <v>3.200000000000003</v>
+        <v>3</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -30.5</t>
+          <t>Kansas State -17.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -29.5</t>
+          <t>Kansas State -17.5</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -32.7</t>
+          <t>Kansas State -20.5</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>32.7</v>
+        <v>20.5</v>
       </c>
       <c r="J36" t="n">
-        <v>29.5</v>
+        <v>17.5</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2156,40 +2156,40 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Michigan State</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Army</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>6.2</v>
+        <v>8.4</v>
       </c>
       <c r="E37" t="n">
         <v>3</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Kansas State -17.5</t>
+          <t>Michigan State -3.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Kansas State -17.5</t>
+          <t>Michigan State -3.5</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Kansas State -20.5</t>
+          <t>Michigan State -0.5</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>20.5</v>
+        <v>0.5</v>
       </c>
       <c r="J37" t="n">
-        <v>17.5</v>
+        <v>3.5</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -2203,40 +2203,40 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Michigan State</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>8.4</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Michigan State -3.5</t>
+          <t>UTSA -4.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Michigan State -3.5</t>
+          <t>UTSA -4.5</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Michigan State -0.5</t>
+          <t>UTSA -1.7</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0.5</v>
+        <v>1.7</v>
       </c>
       <c r="J38" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2250,40 +2250,40 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>8.300000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="E39" t="n">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>UTSA -4.5</t>
+          <t>Virginia Tech -1.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>UTSA -4.5</t>
+          <t>Virginia Tech -1.5</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>UTSA -1.7</t>
+          <t>Virginia Tech -4.1</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1.7</v>
+        <v>4.1</v>
       </c>
       <c r="J39" t="n">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2297,40 +2297,40 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>9.1</v>
+        <v>3.6</v>
       </c>
       <c r="E40" t="n">
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Virginia Tech -1.5</t>
+          <t>Tulsa -3.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Virginia Tech -1.5</t>
+          <t>Tulsa -4.5</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Virginia Tech -4.1</t>
+          <t>Tulsa -6.9</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>4.1</v>
+        <v>-6.9</v>
       </c>
       <c r="J40" t="n">
-        <v>1.5</v>
+        <v>-4.5</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
@@ -2485,40 +2485,40 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="E44" t="n">
-        <v>1.200000000000003</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>LSU -32.5</t>
+          <t>North Carolina -16.5</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>LSU -37.5</t>
+          <t>North Carolina -16.5</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>LSU -36.3</t>
+          <t>North Carolina -17.8</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>36.3</v>
+        <v>-17.8</v>
       </c>
       <c r="J44" t="n">
-        <v>37.5</v>
+        <v>-16.5</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2532,40 +2532,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2.3</v>
+        <v>3.6</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>1.200000000000003</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Nebraska -33.5</t>
+          <t>LSU -32.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Nebraska -34.5</t>
+          <t>LSU -37.5</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Nebraska -33.5</t>
+          <t>LSU -36.3</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>33.5</v>
+        <v>36.3</v>
       </c>
       <c r="J45" t="n">
-        <v>34.5</v>
+        <v>37.5</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
@@ -2579,40 +2579,40 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>9.800000000000001</v>
+        <v>2.3</v>
       </c>
       <c r="E46" t="n">
-        <v>0.8999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Oklahoma -3.0</t>
+          <t>Nebraska -33.5</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Oklahoma -3</t>
+          <t>Nebraska -34.5</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Oklahoma -3.9</t>
+          <t>Nebraska -33.5</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>3.9</v>
+        <v>33.5</v>
       </c>
       <c r="J46" t="n">
-        <v>3</v>
+        <v>34.5</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
@@ -2626,40 +2626,40 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>4.6</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E47" t="n">
-        <v>0.8999999999999986</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Cincinnati -20.5</t>
+          <t>Oklahoma -3.0</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Cincinnati -21.5</t>
+          <t>Oklahoma -3</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cincinnati -20.6</t>
+          <t>Oklahoma -3.9</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>20.6</v>
+        <v>3.9</v>
       </c>
       <c r="J47" t="n">
-        <v>21.5</v>
+        <v>3</v>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
@@ -2673,40 +2673,40 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Duke</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>8.1</v>
+        <v>4.6</v>
       </c>
       <c r="E48" t="n">
-        <v>0.8</v>
+        <v>0.8999999999999986</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Illinois -2.5</t>
+          <t>Cincinnati -20.5</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Illinois -2.5</t>
+          <t>Cincinnati -21.5</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Illinois -1.7</t>
+          <t>Cincinnati -20.6</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>-1.7</v>
+        <v>20.6</v>
       </c>
       <c r="J48" t="n">
-        <v>-2.5</v>
+        <v>21.5</v>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
@@ -2720,40 +2720,40 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>Duke</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>6.2</v>
+        <v>8.1</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1999999999999993</v>
+        <v>0.8</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>BYU -17.5</t>
+          <t>Illinois -2.5</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>BYU -18.5</t>
+          <t>Illinois -2.5</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>BYU -18.7</t>
+          <t>Illinois -1.7</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>18.7</v>
+        <v>-1.7</v>
       </c>
       <c r="J49" t="n">
-        <v>18.5</v>
+        <v>-2.5</v>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
@@ -2767,40 +2767,40 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>James Madison</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>7.6</v>
+        <v>6.2</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Louisville -14.5</t>
+          <t>BYU -17.5</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Louisville -14.5</t>
+          <t>BYU -18.5</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Louisville -14.5</t>
+          <t>BYU -18.7</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>14.5</v>
+        <v>18.7</v>
       </c>
       <c r="J50" t="n">
-        <v>14.5</v>
+        <v>18.5</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
@@ -2814,33 +2814,41 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>James Madison</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="E51" t="inlineStr"/>
+        <v>7.6</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Charlotte -nan</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
+          <t>Louisville -14.5</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Louisville -14.5</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>North Carolina -17.8</t>
+          <t>Louisville -14.5</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>-17.8</v>
-      </c>
-      <c r="J51" t="inlineStr"/>
+        <v>14.5</v>
+      </c>
+      <c r="J51" t="n">
+        <v>14.5</v>
+      </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>

</xml_diff>